<commit_message>
T41 castellated file and memory breakout board
</commit_message>
<xml_diff>
--- a/Teensy 3.6 Touch display LoRa/Teensy 4 Touch Breakout.xlsx
+++ b/Teensy 3.6 Touch display LoRa/Teensy 4 Touch Breakout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Teensy3.1-Breakout-Boards\Teensy 3.6 Touch display LoRa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1762E6D8-0A80-4149-AB77-C2EDD3603563}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAF3474-40BC-4AD2-9C65-3DBDE87D80E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="3000" windowWidth="25485" windowHeight="16725" xr2:uid="{FC75797F-934B-4C08-A1CB-7571A5F80D33}"/>
+    <workbookView xWindow="660" yWindow="3015" windowWidth="20385" windowHeight="17985" xr2:uid="{FC75797F-934B-4C08-A1CB-7571A5F80D33}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="163">
   <si>
     <t>RefDes</t>
   </si>
@@ -978,7 +978,7 @@
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>